<commit_message>
append DATA CONTAS VALOR mesmo se ja tiver sido criado a planilha
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -1385,7 +1385,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="1" sqref="A1:I5 G16"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2030,7 +2030,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="1" sqref="A1:I5 K16"/>
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2652,7 +2652,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="1" sqref="A1:I5 G14"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2804,7 +2804,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="A1:I5"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3069,7 +3069,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M13" activeCellId="1" sqref="A1:I5 M13"/>
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3285,7 +3285,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P16" activeCellId="1" sqref="A1:I5 P16"/>
+      <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3600,17 +3600,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="A1:I5"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3622,16 +3622,6 @@
       <c r="A2" s="64"/>
       <c r="B2" s="65"/>
       <c r="C2" s="66"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3652,7 +3642,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="1" sqref="A1:I5 C21"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3910,7 +3900,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="A1:I5 B20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4343,7 +4333,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="1" sqref="A1:I5 K3"/>
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4640,7 +4630,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="A1:I5 B20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5389,7 +5379,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="1" sqref="A1:I5 M7"/>
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5816,7 +5806,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="A1:I5 E6"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6379,7 +6369,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="1" sqref="A1:I5 F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6636,7 +6626,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="1" sqref="A1:I5 H11"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
codigo atualizado add paciente agr salva no banco de dados marcação, tudo ok
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -1326,7 +1326,16 @@
           <t>C</t>
         </is>
       </c>
-      <c r="I11" s="74" t="n"/>
+      <c r="H11" s="63" t="inlineStr">
+        <is>
+          <t>POLIGLOTA</t>
+        </is>
+      </c>
+      <c r="I11" s="74" t="inlineStr">
+        <is>
+          <t>777777</t>
+        </is>
+      </c>
       <c r="J11" s="75" t="inlineStr">
         <is>
           <t>Total</t>
@@ -1335,6 +1344,11 @@
       <c r="K11" s="76">
         <f>K3+K4+K5+K6+K7+K8+K9+K10</f>
         <v/>
+      </c>
+      <c r="L11" s="63" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="64">
@@ -1578,7 +1592,16 @@
     </row>
     <row r="20" ht="15" customHeight="1" s="64">
       <c r="A20" s="77" t="n"/>
-      <c r="B20" s="78" t="n"/>
+      <c r="B20" s="78" t="inlineStr">
+        <is>
+          <t>POLIGLOTA</t>
+        </is>
+      </c>
+      <c r="C20" s="63" t="inlineStr">
+        <is>
+          <t>777777</t>
+        </is>
+      </c>
       <c r="D20" s="86" t="inlineStr">
         <is>
           <t>Soma</t>
@@ -1587,6 +1610,11 @@
       <c r="E20" s="73">
         <f>E3+E4+E5+E6+E7+E8+E9+E10+E11+E12+E13+E14+E15+E16+E17+E18+E19</f>
         <v/>
+      </c>
+      <c r="F20" s="63" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
       </c>
       <c r="I20" s="87" t="inlineStr">
         <is>
@@ -1601,6 +1629,16 @@
     </row>
     <row r="21" ht="15" customHeight="1" s="64">
       <c r="A21" s="77" t="n"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>JOAO</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
       <c r="D21" s="89" t="inlineStr">
         <is>
           <t>Medico</t>
@@ -1609,6 +1647,11 @@
       <c r="E21" s="90">
         <f>49*17</f>
         <v/>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
       </c>
       <c r="G21" s="29" t="n"/>
       <c r="I21" s="87" t="inlineStr">

</xml_diff>

<commit_message>
atualizado marcação e adicção de pacientes
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -933,7 +933,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
@@ -1342,8 +1342,16 @@
       <c r="G10" s="79" t="n">
         <v>8</v>
       </c>
-      <c r="H10" s="79" t="n"/>
-      <c r="I10" s="76" t="n"/>
+      <c r="H10" s="79" t="inlineStr">
+        <is>
+          <t>CLEBER</t>
+        </is>
+      </c>
+      <c r="I10" s="76" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
       <c r="J10" s="82" t="inlineStr">
         <is>
           <t>Total</t>
@@ -1353,7 +1361,11 @@
         <f>K3+K4+K5+K6+K7+K8+K9+K10</f>
         <v/>
       </c>
-      <c r="L10" s="74" t="n"/>
+      <c r="L10" s="74" t="inlineStr">
+        <is>
+          <t>E:341,26</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="75">
       <c r="A11" s="79" t="n">
@@ -1376,10 +1388,23 @@
           <t>D</t>
         </is>
       </c>
-      <c r="I11" s="85" t="n"/>
+      <c r="H11" s="74" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I11" s="85" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
       <c r="J11" s="86" t="n"/>
       <c r="K11" s="87" t="n"/>
-      <c r="L11" s="74" t="n"/>
+      <c r="L11" s="74" t="inlineStr">
+        <is>
+          <t>D:192,61</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="75">
       <c r="A12" s="79" t="n">
@@ -1403,10 +1428,23 @@
         </is>
       </c>
       <c r="G12" s="88" t="n"/>
-      <c r="H12" s="85" t="n"/>
-      <c r="I12" s="85" t="n"/>
+      <c r="H12" s="85" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="I12" s="85" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
       <c r="J12" s="89" t="n"/>
       <c r="K12" s="14" t="n"/>
+      <c r="L12" s="74" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="75">
       <c r="A13" s="79" t="n">
@@ -1429,14 +1467,23 @@
           <t>E</t>
         </is>
       </c>
-      <c r="H13" s="90" t="n"/>
+      <c r="H13" s="90" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="I13" s="74" t="inlineStr">
         <is>
-          <t>ATEND.MÉDICO</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K13" s="74" t="n">
         <v>2527.05</v>
+      </c>
+      <c r="L13" s="74" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" s="75">
@@ -1460,15 +1507,25 @@
           <t>C</t>
         </is>
       </c>
+      <c r="H14" s="74" t="inlineStr">
+        <is>
+          <t>TTTTTT</t>
+        </is>
+      </c>
       <c r="I14" s="91" t="inlineStr">
         <is>
-          <t>ATEND.PSICOLÓGICO</t>
+          <t>33</t>
         </is>
       </c>
       <c r="J14" s="78" t="n"/>
       <c r="K14" s="92" t="n">
         <v>1540.88</v>
       </c>
+      <c r="L14" s="74" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="75">
       <c r="A15" s="79" t="n">
@@ -1493,15 +1550,25 @@
           <t>C</t>
         </is>
       </c>
+      <c r="H15" s="74" t="inlineStr">
+        <is>
+          <t>SSSSSS</t>
+        </is>
+      </c>
       <c r="I15" s="91" t="inlineStr">
         <is>
-          <t>TOTAL</t>
+          <t>444</t>
         </is>
       </c>
       <c r="J15" s="78" t="n"/>
       <c r="K15" s="18" t="n">
         <v>2378.4</v>
       </c>
+      <c r="L15" s="74" t="inlineStr">
+        <is>
+          <t>C:192,61</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="75">
       <c r="A16" s="79" t="n">
@@ -1524,15 +1591,25 @@
           <t>C</t>
         </is>
       </c>
+      <c r="H16" s="74" t="inlineStr">
+        <is>
+          <t>LUIS</t>
+        </is>
+      </c>
       <c r="I16" s="93" t="inlineStr">
         <is>
-          <t>PAGAM.PSICOLOGA</t>
+          <t>77</t>
         </is>
       </c>
       <c r="J16" s="78" t="n"/>
       <c r="K16" s="94" t="n">
         <v>508</v>
       </c>
+      <c r="L16" s="74" t="inlineStr">
+        <is>
+          <t>E:341,26</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="15" customHeight="1" s="75">
       <c r="A17" s="79" t="n">
@@ -1555,15 +1632,25 @@
           <t>P</t>
         </is>
       </c>
+      <c r="H17" s="74" t="inlineStr">
+        <is>
+          <t>LUCIANO</t>
+        </is>
+      </c>
       <c r="I17" s="91" t="inlineStr">
         <is>
-          <t>PAGAM. MÉDICA</t>
+          <t>444</t>
         </is>
       </c>
       <c r="J17" s="78" t="n"/>
       <c r="K17" s="21" t="n">
         <v>833</v>
       </c>
+      <c r="L17" s="74" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="15" customHeight="1" s="75">
       <c r="A18" s="79" t="n">
@@ -1586,9 +1673,14 @@
           <t>C</t>
         </is>
       </c>
+      <c r="H18" s="74" t="inlineStr">
+        <is>
+          <t>LUIS</t>
+        </is>
+      </c>
       <c r="I18" s="91" t="inlineStr">
         <is>
-          <t>SOMA</t>
+          <t>77</t>
         </is>
       </c>
       <c r="J18" s="78" t="n"/>
@@ -1596,13 +1688,26 @@
         <f>K16-K18-K17</f>
         <v/>
       </c>
+      <c r="L18" s="74" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15" customHeight="1" s="75">
       <c r="A19" s="79" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="79" t="n"/>
-      <c r="C19" s="76" t="n"/>
+      <c r="B19" s="79" t="inlineStr">
+        <is>
+          <t>CLEBER</t>
+        </is>
+      </c>
+      <c r="C19" s="76" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
       <c r="D19" s="82" t="inlineStr">
         <is>
           <t>Soma</t>
@@ -1612,9 +1717,19 @@
         <f>E3+E4+E5+E6+E7+E8+E9+E10+E11+E12+E13+E14+E15+E16+E17+E18+E19</f>
         <v/>
       </c>
+      <c r="F19" s="74" t="inlineStr">
+        <is>
+          <t>E:341,26</t>
+        </is>
+      </c>
+      <c r="H19" s="74" t="inlineStr">
+        <is>
+          <t>ANDRE</t>
+        </is>
+      </c>
       <c r="I19" s="91" t="inlineStr">
         <is>
-          <t>CARTÃO</t>
+          <t>123</t>
         </is>
       </c>
       <c r="J19" s="78" t="n"/>
@@ -1622,10 +1737,24 @@
         <f>E4+E5+E7+E8+E9+E10+E11+E12+E13+E15+E16+E17+E19+K4+K6+K7+K8+K9+K10</f>
         <v/>
       </c>
+      <c r="L19" s="74" t="inlineStr">
+        <is>
+          <t>D:192,61</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="15" customHeight="1" s="75">
       <c r="A20" s="88" t="n"/>
-      <c r="B20" s="89" t="n"/>
+      <c r="B20" s="89" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C20" s="74" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
       <c r="D20" s="97" t="inlineStr">
         <is>
           <t>Medico</t>
@@ -1635,9 +1764,19 @@
         <f>49*17</f>
         <v/>
       </c>
+      <c r="F20" s="74" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
+        </is>
+      </c>
+      <c r="H20" s="74" t="inlineStr">
+        <is>
+          <t>LO</t>
+        </is>
+      </c>
       <c r="I20" s="98" t="inlineStr">
         <is>
-          <t>DINHEIRO</t>
+          <t>25</t>
         </is>
       </c>
       <c r="J20" s="78" t="n"/>
@@ -1645,9 +1784,24 @@
         <f>300+E14</f>
         <v/>
       </c>
+      <c r="L20" s="74" t="inlineStr">
+        <is>
+          <t>D:192,61</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="15" customHeight="1" s="75">
       <c r="A21" s="88" t="n"/>
+      <c r="B21" s="74" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C21" s="74" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="D21" s="100" t="inlineStr">
         <is>
           <t>TOTAL</t>
@@ -1656,10 +1810,20 @@
       <c r="E21" s="101" t="n">
         <v>1444.1</v>
       </c>
+      <c r="F21" s="74" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
+      </c>
       <c r="G21" s="29" t="n"/>
+      <c r="H21" s="74" t="inlineStr">
+        <is>
+          <t>RT</t>
+        </is>
+      </c>
       <c r="I21" s="98" t="inlineStr">
         <is>
-          <t>PIX</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J21" s="78" t="n"/>
@@ -1667,17 +1831,149 @@
         <f>E3+41.26+E18+K3</f>
         <v/>
       </c>
+      <c r="L21" s="74" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="15" customHeight="1" s="75">
       <c r="A22" s="88" t="n"/>
+      <c r="B22" s="74" t="inlineStr">
+        <is>
+          <t>TTTTTT</t>
+        </is>
+      </c>
+      <c r="C22" s="74" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
       <c r="D22" s="100" t="n"/>
       <c r="E22" s="101" t="n"/>
-      <c r="I22" s="102" t="n"/>
+      <c r="F22" s="74" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
+      </c>
+      <c r="H22" s="74" t="inlineStr">
+        <is>
+          <t>LORD</t>
+        </is>
+      </c>
+      <c r="I22" s="102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="J22" s="78" t="n"/>
       <c r="K22" s="103" t="n"/>
+      <c r="L22" s="74" t="inlineStr">
+        <is>
+          <t>C:192,61</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="15" customHeight="1" s="75">
+      <c r="B23" s="74" t="inlineStr">
+        <is>
+          <t>LUIS</t>
+        </is>
+      </c>
+      <c r="C23" s="74" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F23" s="74" t="inlineStr">
+        <is>
+          <t>E:341,26</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>MARCI</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="K23" s="89" t="n"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="74" t="inlineStr">
+        <is>
+          <t>LUCIANO</t>
+        </is>
+      </c>
+      <c r="C24" s="74" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="F24" s="74" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="74" t="inlineStr">
+        <is>
+          <t>LUIS</t>
+        </is>
+      </c>
+      <c r="C25" s="74" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="F25" s="74" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="74" t="inlineStr">
+        <is>
+          <t>RT</t>
+        </is>
+      </c>
+      <c r="C26" s="74" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F26" s="74" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>MARCI</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>C:341,26</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
agora +1 forma de pagamento pede o valor exato
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -2003,8 +2003,8 @@
   </sheetPr>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.11328125" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
@@ -3753,139 +3753,759 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="B2:L6"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.16015625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="44.6" customWidth="1" style="74" min="2" max="2"/>
     <col width="19.36" customWidth="1" style="74" min="6" max="6"/>
+    <col width="37.99" customWidth="1" style="74" min="8" max="8"/>
     <col width="15.81" customWidth="1" style="74" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1" s="75"/>
+    <row r="1" ht="13.5" customHeight="1" s="75">
+      <c r="A1" s="76" t="inlineStr">
+        <is>
+          <t>(CAMPSSA) Atendimento Médico Terça- feira 08/10/2024</t>
+        </is>
+      </c>
+      <c r="B1" s="77" t="n"/>
+      <c r="C1" s="77" t="n"/>
+      <c r="D1" s="77" t="n"/>
+      <c r="E1" s="78" t="n"/>
+      <c r="G1" s="76" t="inlineStr">
+        <is>
+          <t>(CAMPSSA) Atendimento Psicológico Terça-feira 08/10/2024</t>
+        </is>
+      </c>
+      <c r="H1" s="77" t="n"/>
+      <c r="I1" s="77" t="n"/>
+      <c r="J1" s="77" t="n"/>
+      <c r="K1" s="78" t="n"/>
+    </row>
     <row r="2" ht="13.5" customHeight="1" s="75">
-      <c r="C2" s="74" t="n"/>
-      <c r="F2" s="74" t="n"/>
+      <c r="A2" s="79" t="inlineStr">
+        <is>
+          <t>Ordem</t>
+        </is>
+      </c>
+      <c r="B2" s="76" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C2" s="76" t="inlineStr">
+        <is>
+          <t>Renach</t>
+        </is>
+      </c>
+      <c r="D2" s="76" t="inlineStr">
+        <is>
+          <t>Reexames</t>
+        </is>
+      </c>
+      <c r="E2" s="76" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="G2" s="79" t="inlineStr">
+        <is>
+          <t>Ordem</t>
+        </is>
+      </c>
+      <c r="H2" s="76" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="I2" s="76" t="inlineStr">
+        <is>
+          <t>Renach</t>
+        </is>
+      </c>
+      <c r="J2" s="76" t="inlineStr">
+        <is>
+          <t>Reexames</t>
+        </is>
+      </c>
+      <c r="K2" s="76" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="13.5" customHeight="1" s="75">
-      <c r="B3" s="74" t="inlineStr">
-        <is>
-          <t>JOANA</t>
-        </is>
-      </c>
-      <c r="C3" s="74" t="inlineStr">
-        <is>
-          <t>232322</t>
-        </is>
-      </c>
-      <c r="F3" s="74" t="inlineStr">
-        <is>
-          <t>D:300,00 | C:41,26</t>
-        </is>
-      </c>
-      <c r="H3" s="74" t="inlineStr">
-        <is>
-          <t>JOANA</t>
-        </is>
-      </c>
-      <c r="I3" s="74" t="inlineStr">
-        <is>
-          <t>232322</t>
-        </is>
-      </c>
-      <c r="L3" s="74" t="inlineStr">
-        <is>
-          <t>D:300,00 | C:41,26</t>
+      <c r="A3" s="79" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="129" t="inlineStr">
+        <is>
+          <t>LEDA MOREIRA PEIXOTO SANTOS</t>
+        </is>
+      </c>
+      <c r="C3" s="76" t="inlineStr">
+        <is>
+          <t>513881861</t>
+        </is>
+      </c>
+      <c r="D3" s="76" t="n"/>
+      <c r="E3" s="76" t="n"/>
+      <c r="F3" s="89" t="inlineStr">
+        <is>
+          <t>E:148,65</t>
+        </is>
+      </c>
+      <c r="G3" s="79" t="n"/>
+      <c r="H3" s="130" t="inlineStr">
+        <is>
+          <t>HELENA NASCIMENTO ALVAREZ</t>
+        </is>
+      </c>
+      <c r="I3" s="76" t="inlineStr">
+        <is>
+          <t>513870344</t>
+        </is>
+      </c>
+      <c r="J3" s="76" t="n"/>
+      <c r="K3" s="76" t="n"/>
+      <c r="L3" s="89" t="inlineStr">
+        <is>
+          <t>P:341,26</t>
         </is>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1" s="75">
-      <c r="B4" s="74" t="inlineStr">
-        <is>
-          <t>PEDROXA</t>
-        </is>
-      </c>
-      <c r="C4" s="74" t="inlineStr">
-        <is>
-          <t>3243343</t>
-        </is>
-      </c>
-      <c r="F4" s="74" t="inlineStr">
-        <is>
-          <t>C:41,26 | P:300,00</t>
-        </is>
-      </c>
-      <c r="H4" s="74" t="inlineStr">
-        <is>
-          <t>PEDROXA</t>
-        </is>
-      </c>
-      <c r="I4" s="74" t="inlineStr">
-        <is>
-          <t>3243343</t>
-        </is>
-      </c>
-      <c r="L4" s="74" t="inlineStr">
-        <is>
-          <t>C:41,26 | P:300,00</t>
+      <c r="A4" s="79" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="130" t="inlineStr">
+        <is>
+          <t>ALINE BOMFIM DOS SANTOS CRUZ</t>
+        </is>
+      </c>
+      <c r="C4" s="76" t="inlineStr">
+        <is>
+          <t>513887056</t>
+        </is>
+      </c>
+      <c r="D4" s="76" t="n"/>
+      <c r="E4" s="76" t="n"/>
+      <c r="F4" s="89" t="inlineStr">
+        <is>
+          <t>P:148,65</t>
+        </is>
+      </c>
+      <c r="G4" s="79" t="n"/>
+      <c r="H4" s="131" t="inlineStr">
+        <is>
+          <t>RAFAEL LEITE GUIMARAES PIRES</t>
+        </is>
+      </c>
+      <c r="I4" s="76" t="inlineStr">
+        <is>
+          <t>513891672</t>
+        </is>
+      </c>
+      <c r="J4" s="76" t="n"/>
+      <c r="K4" s="76" t="n"/>
+      <c r="L4" s="89" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
         </is>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1" s="75">
-      <c r="B5" s="74" t="inlineStr">
-        <is>
-          <t>FFRRG</t>
-        </is>
-      </c>
-      <c r="C5" s="74" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
-      </c>
-      <c r="F5" s="74" t="inlineStr">
-        <is>
-          <t>D:300,00 | E:41,26</t>
-        </is>
-      </c>
-      <c r="H5" s="74" t="inlineStr">
-        <is>
-          <t>FFRRG</t>
-        </is>
-      </c>
-      <c r="I5" s="74" t="inlineStr">
-        <is>
-          <t>3333</t>
-        </is>
-      </c>
-      <c r="L5" s="74" t="inlineStr">
-        <is>
-          <t>D:300,00 | E:41,26</t>
+      <c r="A5" s="79" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="131" t="inlineStr">
+        <is>
+          <t>HELENA NASCIMENTO ALVAREZ</t>
+        </is>
+      </c>
+      <c r="C5" s="76" t="inlineStr">
+        <is>
+          <t>513870344</t>
+        </is>
+      </c>
+      <c r="D5" s="76" t="n"/>
+      <c r="E5" s="76" t="n"/>
+      <c r="F5" s="89" t="inlineStr">
+        <is>
+          <t>P:341,26</t>
+        </is>
+      </c>
+      <c r="G5" s="79" t="n"/>
+      <c r="H5" s="131" t="inlineStr">
+        <is>
+          <t>ASSSDD</t>
+        </is>
+      </c>
+      <c r="I5" s="76" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="J5" s="76" t="n"/>
+      <c r="K5" s="76" t="n"/>
+      <c r="L5" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,27</t>
         </is>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="75">
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>SSSSS</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>4444</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>E:100,00 | P:92,61</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="13.5" customHeight="1" s="75"/>
+      <c r="A6" s="79" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="132" t="inlineStr">
+        <is>
+          <t>NEUZA DE SOUZA CAVALCANTI ARAUJO</t>
+        </is>
+      </c>
+      <c r="C6" s="76" t="inlineStr">
+        <is>
+          <t>014100697</t>
+        </is>
+      </c>
+      <c r="D6" s="76" t="n"/>
+      <c r="E6" s="76" t="n"/>
+      <c r="F6" s="89" t="inlineStr">
+        <is>
+          <t>E:148,65</t>
+        </is>
+      </c>
+      <c r="G6" s="79" t="n"/>
+      <c r="H6" s="131" t="inlineStr">
+        <is>
+          <t>ASDD</t>
+        </is>
+      </c>
+      <c r="I6" s="76" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="J6" s="76" t="n"/>
+      <c r="K6" s="76" t="n"/>
+      <c r="L6" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,27</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="13.5" customHeight="1" s="75">
+      <c r="A7" s="79" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="131" t="inlineStr">
+        <is>
+          <t>RAFAEL LEITE GUIMARAES PIRES</t>
+        </is>
+      </c>
+      <c r="C7" s="76" t="inlineStr">
+        <is>
+          <t>513891672</t>
+        </is>
+      </c>
+      <c r="D7" s="76" t="n"/>
+      <c r="E7" s="76" t="n"/>
+      <c r="F7" s="89" t="inlineStr">
+        <is>
+          <t>D:341,26</t>
+        </is>
+      </c>
+      <c r="G7" s="79" t="n"/>
+      <c r="H7" s="131" t="inlineStr">
+        <is>
+          <t>DWAD</t>
+        </is>
+      </c>
+      <c r="I7" s="76" t="inlineStr">
+        <is>
+          <t>322323</t>
+        </is>
+      </c>
+      <c r="J7" s="76" t="n"/>
+      <c r="K7" s="76" t="n"/>
+      <c r="L7" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,27</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="13.5" customHeight="1" s="75">
+      <c r="A8" s="79" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="132" t="inlineStr">
+        <is>
+          <t>NACKSON GOMES FONSECA</t>
+        </is>
+      </c>
+      <c r="C8" s="76" t="inlineStr">
+        <is>
+          <t>513874709</t>
+        </is>
+      </c>
+      <c r="D8" s="76" t="n"/>
+      <c r="E8" s="76" t="n"/>
+      <c r="F8" s="89" t="inlineStr">
+        <is>
+          <t>D:148,65</t>
+        </is>
+      </c>
+      <c r="G8" s="79" t="n"/>
+      <c r="H8" s="131" t="inlineStr">
+        <is>
+          <t>SASAS</t>
+        </is>
+      </c>
+      <c r="I8" s="76" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
+      <c r="J8" s="76" t="n"/>
+      <c r="K8" s="76" t="n"/>
+      <c r="L8" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,26</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="13.5" customHeight="1" s="75">
+      <c r="A9" s="79" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="131" t="inlineStr">
+        <is>
+          <t>PEDRO HENRIQUE CUNHA LEITE</t>
+        </is>
+      </c>
+      <c r="C9" s="76" t="inlineStr">
+        <is>
+          <t>513861471</t>
+        </is>
+      </c>
+      <c r="D9" s="76" t="n"/>
+      <c r="E9" s="76" t="n"/>
+      <c r="F9" s="89" t="inlineStr">
+        <is>
+          <t>C:148,65</t>
+        </is>
+      </c>
+      <c r="G9" s="79" t="n"/>
+      <c r="H9" s="131" t="n"/>
+      <c r="I9" s="76" t="n"/>
+      <c r="J9" s="76" t="n"/>
+      <c r="K9" s="76" t="n"/>
+      <c r="L9" s="89" t="n"/>
+    </row>
+    <row r="10" ht="13.5" customHeight="1" s="75">
+      <c r="A10" s="79" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="131" t="inlineStr">
+        <is>
+          <t>EDUARDA DE PAULA SAMPAIO</t>
+        </is>
+      </c>
+      <c r="C10" s="76" t="inlineStr">
+        <is>
+          <t>513874599</t>
+        </is>
+      </c>
+      <c r="D10" s="76" t="n"/>
+      <c r="E10" s="76" t="n"/>
+      <c r="F10" s="89" t="inlineStr">
+        <is>
+          <t>C:148,65</t>
+        </is>
+      </c>
+      <c r="G10" s="79" t="n"/>
+      <c r="H10" s="81" t="n"/>
+      <c r="I10" s="76" t="n"/>
+      <c r="J10" s="76" t="n"/>
+      <c r="K10" s="76" t="n"/>
+      <c r="L10" s="89" t="n"/>
+    </row>
+    <row r="11" ht="13.5" customHeight="1" s="75">
+      <c r="A11" s="79" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="131" t="inlineStr">
+        <is>
+          <t>LAERTE ALVES SANTOS</t>
+        </is>
+      </c>
+      <c r="C11" s="76" t="inlineStr">
+        <is>
+          <t>513824087</t>
+        </is>
+      </c>
+      <c r="D11" s="76" t="n"/>
+      <c r="E11" s="76" t="n"/>
+      <c r="F11" s="89" t="inlineStr">
+        <is>
+          <t>E:148,65</t>
+        </is>
+      </c>
+      <c r="G11" s="79" t="n"/>
+      <c r="H11" s="81" t="n"/>
+      <c r="I11" s="76" t="n"/>
+      <c r="J11" s="76" t="n"/>
+      <c r="K11" s="76" t="n"/>
+      <c r="L11" s="89" t="n"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1" s="75">
+      <c r="A12" s="79" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="131" t="inlineStr">
+        <is>
+          <t>MARCOS VINICIUS DANTAS CANARIO</t>
+        </is>
+      </c>
+      <c r="C12" s="76" t="inlineStr">
+        <is>
+          <t>513726526</t>
+        </is>
+      </c>
+      <c r="D12" s="76" t="n"/>
+      <c r="E12" s="76" t="n"/>
+      <c r="F12" s="89" t="inlineStr">
+        <is>
+          <t>P:148,65</t>
+        </is>
+      </c>
+      <c r="G12" s="79" t="n"/>
+      <c r="H12" s="81" t="n"/>
+      <c r="I12" s="76" t="n"/>
+      <c r="J12" s="76" t="n"/>
+      <c r="K12" s="76" t="n"/>
+      <c r="L12" s="89" t="n"/>
+    </row>
+    <row r="13" ht="13.5" customHeight="1" s="75">
+      <c r="A13" s="79" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="131" t="inlineStr">
+        <is>
+          <t>MAYRA AUGUSTO MEDEIROS</t>
+        </is>
+      </c>
+      <c r="C13" s="76" t="inlineStr">
+        <is>
+          <t>513875664</t>
+        </is>
+      </c>
+      <c r="D13" s="76" t="n"/>
+      <c r="E13" s="76" t="n"/>
+      <c r="F13" s="89" t="inlineStr">
+        <is>
+          <t>C:148,65</t>
+        </is>
+      </c>
+      <c r="G13" s="89" t="n"/>
+      <c r="H13" s="89" t="n"/>
+      <c r="I13" s="85" t="n"/>
+      <c r="J13" s="86" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K13" s="87">
+        <f>K3+K4+K5+K6+K7+K8+K9+K10+K11+K12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" ht="13.5" customHeight="1" s="75">
+      <c r="A14" s="79" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="131" t="inlineStr">
+        <is>
+          <t>MIRIAM CARNEIRO LIMA</t>
+        </is>
+      </c>
+      <c r="C14" s="76" t="inlineStr">
+        <is>
+          <t>513894813</t>
+        </is>
+      </c>
+      <c r="D14" s="76" t="n"/>
+      <c r="E14" s="76" t="n"/>
+      <c r="F14" s="89" t="inlineStr">
+        <is>
+          <t>C:148,65</t>
+        </is>
+      </c>
+      <c r="G14" s="88" t="n"/>
+      <c r="H14" s="85" t="n"/>
+      <c r="I14" s="85" t="n"/>
+      <c r="J14" s="89" t="n"/>
+      <c r="K14" s="14" t="n"/>
+    </row>
+    <row r="15" ht="13.5" customHeight="1" s="75">
+      <c r="A15" s="79" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="131" t="inlineStr">
+        <is>
+          <t>ALBERTO CESAR DE ARAUJO LEAL</t>
+        </is>
+      </c>
+      <c r="C15" s="76" t="inlineStr">
+        <is>
+          <t>513870271</t>
+        </is>
+      </c>
+      <c r="D15" s="76" t="n"/>
+      <c r="E15" s="76" t="n"/>
+      <c r="F15" s="89" t="inlineStr">
+        <is>
+          <t>D:148,65</t>
+        </is>
+      </c>
+      <c r="H15" s="90" t="n"/>
+      <c r="I15" s="74" t="n"/>
+      <c r="K15" s="74" t="n"/>
+    </row>
+    <row r="16" ht="13.5" customHeight="1" s="75">
+      <c r="A16" s="79" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="81" t="inlineStr">
+        <is>
+          <t>SORAIA PONDE AVENA</t>
+        </is>
+      </c>
+      <c r="C16" s="76" t="inlineStr">
+        <is>
+          <t>513842138</t>
+        </is>
+      </c>
+      <c r="D16" s="76" t="n"/>
+      <c r="E16" s="76" t="n"/>
+      <c r="F16" s="89" t="inlineStr">
+        <is>
+          <t>E:148,65</t>
+        </is>
+      </c>
+      <c r="I16" s="91" t="n"/>
+      <c r="J16" s="78" t="n"/>
+      <c r="K16" s="92" t="n"/>
+    </row>
+    <row r="17" ht="13.5" customHeight="1" s="75">
+      <c r="A17" s="79" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="81" t="inlineStr">
+        <is>
+          <t>ICARO ARON SOUZA BASTOS</t>
+        </is>
+      </c>
+      <c r="C17" s="76" t="inlineStr">
+        <is>
+          <t>513900047</t>
+        </is>
+      </c>
+      <c r="D17" s="76" t="n"/>
+      <c r="E17" s="76" t="n"/>
+      <c r="F17" s="89" t="inlineStr">
+        <is>
+          <t>C:148,65</t>
+        </is>
+      </c>
+      <c r="I17" s="91" t="n"/>
+      <c r="J17" s="78" t="n"/>
+      <c r="K17" s="92" t="n"/>
+    </row>
+    <row r="18" ht="13.5" customHeight="1" s="75">
+      <c r="A18" s="79" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="81" t="inlineStr">
+        <is>
+          <t>ELLEN CRISTINA RAMOS PENA</t>
+        </is>
+      </c>
+      <c r="C18" s="76" t="inlineStr">
+        <is>
+          <t>513792494</t>
+        </is>
+      </c>
+      <c r="D18" s="76" t="n"/>
+      <c r="E18" s="76" t="n"/>
+      <c r="F18" s="89" t="inlineStr">
+        <is>
+          <t>C:148,65</t>
+        </is>
+      </c>
+      <c r="I18" s="93" t="n"/>
+      <c r="J18" s="78" t="n"/>
+      <c r="K18" s="94" t="n"/>
+    </row>
+    <row r="19" ht="13.5" customHeight="1" s="75">
+      <c r="A19" s="79" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="81" t="inlineStr">
+        <is>
+          <t>ASSSDD</t>
+        </is>
+      </c>
+      <c r="C19" s="76" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="D19" s="76" t="n"/>
+      <c r="E19" s="76" t="n"/>
+      <c r="F19" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,27</t>
+        </is>
+      </c>
+      <c r="I19" s="91" t="n"/>
+      <c r="J19" s="78" t="n"/>
+      <c r="K19" s="21" t="n"/>
+    </row>
+    <row r="20" ht="13.5" customHeight="1" s="75">
+      <c r="A20" s="79" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="81" t="inlineStr">
+        <is>
+          <t>ASDD</t>
+        </is>
+      </c>
+      <c r="C20" s="76" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="D20" s="76" t="n"/>
+      <c r="E20" s="76" t="n"/>
+      <c r="F20" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,27</t>
+        </is>
+      </c>
+      <c r="I20" s="91" t="n"/>
+      <c r="J20" s="78" t="n"/>
+      <c r="K20" s="95" t="n"/>
+    </row>
+    <row r="21" ht="13.5" customHeight="1" s="75">
+      <c r="A21" s="79" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="81" t="inlineStr">
+        <is>
+          <t>DWAD</t>
+        </is>
+      </c>
+      <c r="C21" s="76" t="inlineStr">
+        <is>
+          <t>322323</t>
+        </is>
+      </c>
+      <c r="D21" s="76" t="n"/>
+      <c r="E21" s="76" t="n"/>
+      <c r="F21" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,27</t>
+        </is>
+      </c>
+      <c r="I21" s="91" t="n"/>
+      <c r="J21" s="78" t="n"/>
+      <c r="K21" s="96" t="n"/>
+    </row>
+    <row r="22" ht="13.5" customHeight="1" s="75">
+      <c r="A22" s="79" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" s="81" t="inlineStr">
+        <is>
+          <t>SASAS</t>
+        </is>
+      </c>
+      <c r="C22" s="76" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
+      <c r="D22" s="76" t="n"/>
+      <c r="E22" s="76" t="n"/>
+      <c r="F22" s="89" t="inlineStr">
+        <is>
+          <t>E:300,00 | P:41,26</t>
+        </is>
+      </c>
+      <c r="I22" s="98" t="n"/>
+      <c r="J22" s="78" t="n"/>
+      <c r="K22" s="99" t="n"/>
+    </row>
+    <row r="23" ht="13.5" customHeight="1" s="75">
+      <c r="A23" s="79" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" s="81" t="n"/>
+      <c r="C23" s="133" t="n"/>
+      <c r="D23" s="76" t="n"/>
+      <c r="E23" s="76" t="n"/>
+      <c r="F23" s="89" t="n"/>
+      <c r="G23" s="29" t="n"/>
+      <c r="I23" s="98" t="n"/>
+      <c r="J23" s="78" t="n"/>
+      <c r="K23" s="99" t="n"/>
+    </row>
+    <row r="24" ht="13.5" customHeight="1" s="75">
+      <c r="A24" s="88" t="n"/>
+      <c r="B24" s="89" t="n"/>
+      <c r="C24" s="74" t="n"/>
+      <c r="D24" s="97" t="n"/>
+      <c r="E24" s="84" t="n"/>
+      <c r="I24" s="102" t="n"/>
+      <c r="J24" s="78" t="n"/>
+      <c r="K24" s="103" t="n"/>
+    </row>
+    <row r="25" ht="13.5" customHeight="1" s="75">
+      <c r="A25" s="88" t="n"/>
+      <c r="C25" s="74" t="n"/>
+      <c r="D25" s="100" t="n"/>
+      <c r="E25" s="101" t="n"/>
+      <c r="I25" s="74" t="n"/>
+      <c r="K25" s="74" t="n"/>
+    </row>
+    <row r="26" ht="13.5" customHeight="1" s="75">
+      <c r="A26" s="88" t="n"/>
+      <c r="C26" s="74" t="n"/>
+      <c r="D26" s="100" t="n"/>
+      <c r="E26" s="101" t="n"/>
+      <c r="I26" s="74" t="n"/>
+      <c r="K26" s="74" t="n"/>
+    </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+  </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
codigo melhorado, funções removidas, nova class acrescentada para validar informações pagamentos etc
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -4101,11 +4101,23 @@
         </is>
       </c>
       <c r="G9" s="79" t="n"/>
-      <c r="H9" s="131" t="n"/>
-      <c r="I9" s="76" t="n"/>
+      <c r="H9" s="131" t="inlineStr">
+        <is>
+          <t>ASDAASDDAS</t>
+        </is>
+      </c>
+      <c r="I9" s="76" t="inlineStr">
+        <is>
+          <t>32243423</t>
+        </is>
+      </c>
       <c r="J9" s="76" t="n"/>
       <c r="K9" s="76" t="n"/>
-      <c r="L9" s="89" t="n"/>
+      <c r="L9" s="89" t="inlineStr">
+        <is>
+          <t>E:R$ 300,00 | P:R$ 41,27</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="13.5" customHeight="1" s="75">
       <c r="A10" s="79" t="n">
@@ -4129,11 +4141,23 @@
         </is>
       </c>
       <c r="G10" s="79" t="n"/>
-      <c r="H10" s="81" t="n"/>
-      <c r="I10" s="76" t="n"/>
+      <c r="H10" s="81" t="inlineStr">
+        <is>
+          <t>SDADDSS</t>
+        </is>
+      </c>
+      <c r="I10" s="76" t="inlineStr">
+        <is>
+          <t>3232323</t>
+        </is>
+      </c>
       <c r="J10" s="76" t="n"/>
       <c r="K10" s="76" t="n"/>
-      <c r="L10" s="89" t="n"/>
+      <c r="L10" s="89" t="inlineStr">
+        <is>
+          <t>E:R$ 300,00 | P:R$ 41,26</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="13.5" customHeight="1" s="75">
       <c r="A11" s="79" t="n">
@@ -4456,11 +4480,23 @@
       <c r="A23" s="79" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="81" t="n"/>
-      <c r="C23" s="133" t="n"/>
+      <c r="B23" s="81" t="inlineStr">
+        <is>
+          <t>ASDAASDDAS</t>
+        </is>
+      </c>
+      <c r="C23" s="133" t="inlineStr">
+        <is>
+          <t>32243423</t>
+        </is>
+      </c>
       <c r="D23" s="76" t="n"/>
       <c r="E23" s="76" t="n"/>
-      <c r="F23" s="89" t="n"/>
+      <c r="F23" s="89" t="inlineStr">
+        <is>
+          <t>E:R$ 300,00 | P:R$ 41,27</t>
+        </is>
+      </c>
       <c r="G23" s="29" t="n"/>
       <c r="I23" s="98" t="n"/>
       <c r="J23" s="78" t="n"/>
@@ -4468,10 +4504,23 @@
     </row>
     <row r="24" ht="13.5" customHeight="1" s="75">
       <c r="A24" s="88" t="n"/>
-      <c r="B24" s="89" t="n"/>
-      <c r="C24" s="74" t="n"/>
+      <c r="B24" s="89" t="inlineStr">
+        <is>
+          <t>SDADDSS</t>
+        </is>
+      </c>
+      <c r="C24" s="74" t="inlineStr">
+        <is>
+          <t>3232323</t>
+        </is>
+      </c>
       <c r="D24" s="97" t="n"/>
       <c r="E24" s="84" t="n"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>E:R$ 300,00 | P:R$ 41,26</t>
+        </is>
+      </c>
       <c r="I24" s="102" t="n"/>
       <c r="J24" s="78" t="n"/>
       <c r="K24" s="103" t="n"/>

</xml_diff>

<commit_message>
exibir informação nao muda mais a cor do codigo inteiro
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="01.10" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Planilha13" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Contas Fechamento" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Planilha15" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="sheet nova" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -3817,21 +3818,21 @@
           <t>(Usuário) Atendimento Médico 18/11/2024</t>
         </is>
       </c>
-      <c r="B1" s="144" t="n"/>
-      <c r="C1" s="144" t="n"/>
-      <c r="D1" s="144" t="n"/>
-      <c r="E1" s="144" t="n"/>
-      <c r="F1" s="145" t="n"/>
+      <c r="B1" s="77" t="n"/>
+      <c r="C1" s="77" t="n"/>
+      <c r="D1" s="77" t="n"/>
+      <c r="E1" s="77" t="n"/>
+      <c r="F1" s="78" t="n"/>
       <c r="G1" s="143" t="inlineStr">
         <is>
           <t>(Usuário) Atendimento Psicológico 18/11/2024</t>
         </is>
       </c>
-      <c r="H1" s="144" t="n"/>
-      <c r="I1" s="144" t="n"/>
-      <c r="J1" s="144" t="n"/>
-      <c r="K1" s="144" t="n"/>
-      <c r="L1" s="145" t="n"/>
+      <c r="H1" s="77" t="n"/>
+      <c r="I1" s="77" t="n"/>
+      <c r="J1" s="77" t="n"/>
+      <c r="K1" s="77" t="n"/>
+      <c r="L1" s="78" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="143" t="inlineStr">
@@ -4295,6 +4296,227 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="8" customWidth="1" style="75" min="1" max="1"/>
+    <col width="40" customWidth="1" style="75" min="2" max="2"/>
+    <col width="12" customWidth="1" style="75" min="3" max="3"/>
+    <col width="12" customWidth="1" style="75" min="4" max="4"/>
+    <col width="12" customWidth="1" style="75" min="5" max="5"/>
+    <col width="15" customWidth="1" style="75" min="6" max="6"/>
+    <col width="8" customWidth="1" style="75" min="7" max="7"/>
+    <col width="40" customWidth="1" style="75" min="8" max="8"/>
+    <col width="12" customWidth="1" style="75" min="9" max="9"/>
+    <col width="12" customWidth="1" style="75" min="10" max="10"/>
+    <col width="12" customWidth="1" style="75" min="11" max="11"/>
+    <col width="15" customWidth="1" style="75" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="143" t="inlineStr">
+        <is>
+          <t>(Usuário) Atendimento Médico 18/11/2024</t>
+        </is>
+      </c>
+      <c r="B1" s="144" t="n"/>
+      <c r="C1" s="144" t="n"/>
+      <c r="D1" s="144" t="n"/>
+      <c r="E1" s="144" t="n"/>
+      <c r="F1" s="145" t="n"/>
+      <c r="G1" s="143" t="inlineStr">
+        <is>
+          <t>(Usuário) Atendimento Psicológico 18/11/2024</t>
+        </is>
+      </c>
+      <c r="H1" s="144" t="n"/>
+      <c r="I1" s="144" t="n"/>
+      <c r="J1" s="144" t="n"/>
+      <c r="K1" s="144" t="n"/>
+      <c r="L1" s="145" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="143" t="inlineStr">
+        <is>
+          <t>Ordem</t>
+        </is>
+      </c>
+      <c r="B2" s="143" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C2" s="143" t="inlineStr">
+        <is>
+          <t>Renach</t>
+        </is>
+      </c>
+      <c r="D2" s="143" t="inlineStr">
+        <is>
+          <t>Reexames</t>
+        </is>
+      </c>
+      <c r="E2" s="143" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="F2" s="143" t="inlineStr">
+        <is>
+          <t>Pagamento</t>
+        </is>
+      </c>
+      <c r="G2" s="143" t="inlineStr">
+        <is>
+          <t>Ordem</t>
+        </is>
+      </c>
+      <c r="H2" s="143" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="I2" s="143" t="inlineStr">
+        <is>
+          <t>Renach</t>
+        </is>
+      </c>
+      <c r="J2" s="143" t="inlineStr">
+        <is>
+          <t>Reexames</t>
+        </is>
+      </c>
+      <c r="K2" s="143" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="L2" s="143" t="inlineStr">
+        <is>
+          <t>Pagamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="146" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="147" t="inlineStr">
+        <is>
+          <t>DSSSD</t>
+        </is>
+      </c>
+      <c r="C3" s="146" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="D3" s="146" t="inlineStr"/>
+      <c r="E3" s="148" t="n">
+        <v>148.65</v>
+      </c>
+      <c r="F3" s="146" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="G3" s="146" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="147" t="inlineStr">
+        <is>
+          <t>DSSSD</t>
+        </is>
+      </c>
+      <c r="I3" s="146" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="J3" s="146" t="inlineStr"/>
+      <c r="K3" s="148" t="n">
+        <v>192.61</v>
+      </c>
+      <c r="L3" s="146" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Soma</t>
+        </is>
+      </c>
+      <c r="E4" s="149" t="n">
+        <v>148.65</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Soma</t>
+        </is>
+      </c>
+      <c r="K4" s="149" t="n">
+        <v>192.61</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Médico</t>
+        </is>
+      </c>
+      <c r="E5" s="149" t="n">
+        <v>49</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Psicólogo</t>
+        </is>
+      </c>
+      <c r="K5" s="149" t="n">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E6" s="149" t="n">
+        <v>99.65000000000001</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K6" s="149" t="n">
+        <v>129.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
codigos do banco att
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -5733,7 +5733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
@@ -5761,21 +5761,21 @@
           <t>(Usuário) Atendimento Médico 18/11/2024</t>
         </is>
       </c>
-      <c r="B1" s="150" t="n"/>
-      <c r="C1" s="150" t="n"/>
-      <c r="D1" s="150" t="n"/>
-      <c r="E1" s="150" t="n"/>
-      <c r="F1" s="151" t="n"/>
+      <c r="B1" s="80" t="n"/>
+      <c r="C1" s="80" t="n"/>
+      <c r="D1" s="80" t="n"/>
+      <c r="E1" s="80" t="n"/>
+      <c r="F1" s="81" t="n"/>
       <c r="G1" s="149" t="inlineStr">
         <is>
           <t>(Usuário) Atendimento Psicológico 18/11/2024</t>
         </is>
       </c>
-      <c r="H1" s="150" t="n"/>
-      <c r="I1" s="150" t="n"/>
-      <c r="J1" s="150" t="n"/>
-      <c r="K1" s="150" t="n"/>
-      <c r="L1" s="151" t="n"/>
+      <c r="H1" s="80" t="n"/>
+      <c r="I1" s="80" t="n"/>
+      <c r="J1" s="80" t="n"/>
+      <c r="K1" s="80" t="n"/>
+      <c r="L1" s="81" t="n"/>
     </row>
     <row r="2" ht="15" customHeight="1" s="78">
       <c r="A2" s="149" t="inlineStr">
@@ -5913,12 +5913,12 @@
       </c>
       <c r="H4" s="153" t="inlineStr">
         <is>
-          <t>GABRIEL CARNEIRO FERNANDES</t>
+          <t>ALICE DOS SANTOS RODRIGUES</t>
         </is>
       </c>
       <c r="I4" s="152" t="inlineStr">
         <is>
-          <t>513733841</t>
+          <t>14090930</t>
         </is>
       </c>
       <c r="J4" s="152" t="inlineStr"/>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="L4" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -5937,12 +5937,12 @@
       </c>
       <c r="B5" s="153" t="inlineStr">
         <is>
-          <t>GABRIEL CARNEIRO FERNANDES</t>
+          <t>HAROLDO MASCARENHAS DOS SANTOS</t>
         </is>
       </c>
       <c r="C5" s="152" t="inlineStr">
         <is>
-          <t>513733841</t>
+          <t>513709344</t>
         </is>
       </c>
       <c r="D5" s="152" t="inlineStr"/>
@@ -5951,7 +5951,7 @@
       </c>
       <c r="F5" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G5" s="152" t="n">
@@ -5959,12 +5959,12 @@
       </c>
       <c r="H5" s="153" t="inlineStr">
         <is>
-          <t>ALICE DOS SANTOS RODRIGUES</t>
+          <t>NEUVANIA GONCALVES FERNANDES</t>
         </is>
       </c>
       <c r="I5" s="152" t="inlineStr">
         <is>
-          <t>14090930</t>
+          <t>513784410</t>
         </is>
       </c>
       <c r="J5" s="152" t="inlineStr"/>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="L5" s="152" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
     </row>
@@ -5983,12 +5983,12 @@
       </c>
       <c r="B6" s="153" t="inlineStr">
         <is>
-          <t>HAROLDO MASCARENHAS DOS SANTOS</t>
+          <t>RODRIGO DE OLIVEIRA MOITINHO SANTOS</t>
         </is>
       </c>
       <c r="C6" s="152" t="inlineStr">
         <is>
-          <t>513709344</t>
+          <t>513783161</t>
         </is>
       </c>
       <c r="D6" s="152" t="inlineStr"/>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="F6" s="152" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>P</t>
         </is>
       </c>
       <c r="G6" s="152" t="n">
@@ -6005,12 +6005,12 @@
       </c>
       <c r="H6" s="153" t="inlineStr">
         <is>
-          <t>NEUVANIA GONCALVES FERNANDES</t>
+          <t>RODRIGO SANTOS SILVA</t>
         </is>
       </c>
       <c r="I6" s="152" t="inlineStr">
         <is>
-          <t>513784410</t>
+          <t>513790094</t>
         </is>
       </c>
       <c r="J6" s="152" t="inlineStr"/>
@@ -6029,12 +6029,12 @@
       </c>
       <c r="B7" s="153" t="inlineStr">
         <is>
-          <t>RODRIGO DE OLIVEIRA MOITINHO SANTOS</t>
+          <t>ALICE DOS SANTOS RODRIGUES</t>
         </is>
       </c>
       <c r="C7" s="152" t="inlineStr">
         <is>
-          <t>513783161</t>
+          <t>14090930</t>
         </is>
       </c>
       <c r="D7" s="152" t="inlineStr"/>
@@ -6043,7 +6043,7 @@
       </c>
       <c r="F7" s="152" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G7" s="152" t="n">
@@ -6051,12 +6051,12 @@
       </c>
       <c r="H7" s="153" t="inlineStr">
         <is>
-          <t>RODRIGO SANTOS SILVA</t>
+          <t>RAIANE DE SOUZA DANTAS</t>
         </is>
       </c>
       <c r="I7" s="152" t="inlineStr">
         <is>
-          <t>513790094</t>
+          <t>513608124</t>
         </is>
       </c>
       <c r="J7" s="152" t="inlineStr"/>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="L7" s="152" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -6075,12 +6075,12 @@
       </c>
       <c r="B8" s="153" t="inlineStr">
         <is>
-          <t>ALICE DOS SANTOS RODRIGUES</t>
+          <t>NEUVANIA GONCALVES FERNANDES</t>
         </is>
       </c>
       <c r="C8" s="152" t="inlineStr">
         <is>
-          <t>14090930</t>
+          <t>513784410</t>
         </is>
       </c>
       <c r="D8" s="152" t="inlineStr"/>
@@ -6089,7 +6089,7 @@
       </c>
       <c r="F8" s="152" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="G8" s="152" t="n">
@@ -6097,12 +6097,12 @@
       </c>
       <c r="H8" s="153" t="inlineStr">
         <is>
-          <t>RAIANE DE SOUZA DANTAS</t>
+          <t>JURGEN WILLI LUDWIG VONNEILICH</t>
         </is>
       </c>
       <c r="I8" s="152" t="inlineStr">
         <is>
-          <t>513608124</t>
+          <t>513762567</t>
         </is>
       </c>
       <c r="J8" s="152" t="inlineStr"/>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="L8" s="152" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -6121,12 +6121,12 @@
       </c>
       <c r="B9" s="153" t="inlineStr">
         <is>
-          <t>NEUVANIA GONCALVES FERNANDES</t>
+          <t>ANTONIO JOSE PAMPONET BITTENCOURT</t>
         </is>
       </c>
       <c r="C9" s="152" t="inlineStr">
         <is>
-          <t>513784410</t>
+          <t>513793384</t>
         </is>
       </c>
       <c r="D9" s="152" t="inlineStr"/>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="F9" s="152" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G9" s="152" t="n">
@@ -6143,12 +6143,12 @@
       </c>
       <c r="H9" s="153" t="inlineStr">
         <is>
-          <t>JURGEN WILLI LUDWIG VONNEILICH</t>
+          <t>MOISES SANTOS DA SILVA</t>
         </is>
       </c>
       <c r="I9" s="152" t="inlineStr">
         <is>
-          <t>513762567</t>
+          <t>513760379</t>
         </is>
       </c>
       <c r="J9" s="152" t="inlineStr"/>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="L9" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -6167,12 +6167,12 @@
       </c>
       <c r="B10" s="153" t="inlineStr">
         <is>
-          <t>ANTONIO JOSE PAMPONET BITTENCOURT</t>
+          <t>RODRIGO SANTOS SILVA</t>
         </is>
       </c>
       <c r="C10" s="152" t="inlineStr">
         <is>
-          <t>513793384</t>
+          <t>513790094</t>
         </is>
       </c>
       <c r="D10" s="152" t="inlineStr"/>
@@ -6181,7 +6181,7 @@
       </c>
       <c r="F10" s="152" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="G10" s="152" t="n">
@@ -6189,12 +6189,12 @@
       </c>
       <c r="H10" s="153" t="inlineStr">
         <is>
-          <t>MOISES SANTOS DA SILVA</t>
+          <t>LUCAS CERQUEIRA BATISTA</t>
         </is>
       </c>
       <c r="I10" s="152" t="inlineStr">
         <is>
-          <t>513760379</t>
+          <t>513782331</t>
         </is>
       </c>
       <c r="J10" s="152" t="inlineStr"/>
@@ -6203,7 +6203,7 @@
       </c>
       <c r="L10" s="152" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -6213,12 +6213,12 @@
       </c>
       <c r="B11" s="153" t="inlineStr">
         <is>
-          <t>RODRIGO SANTOS SILVA</t>
+          <t>RAIANE DE SOUZA DANTAS</t>
         </is>
       </c>
       <c r="C11" s="152" t="inlineStr">
         <is>
-          <t>513790094</t>
+          <t>513608124</t>
         </is>
       </c>
       <c r="D11" s="152" t="inlineStr"/>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="F11" s="152" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G11" s="152" t="n">
@@ -6235,12 +6235,12 @@
       </c>
       <c r="H11" s="153" t="inlineStr">
         <is>
-          <t>LUCAS CERQUEIRA BATISTA</t>
+          <t>MARIVALDO ARAGAO FERREIRA</t>
         </is>
       </c>
       <c r="I11" s="152" t="inlineStr">
         <is>
-          <t>513782331</t>
+          <t>513775191</t>
         </is>
       </c>
       <c r="J11" s="152" t="inlineStr"/>
@@ -6259,12 +6259,12 @@
       </c>
       <c r="B12" s="153" t="inlineStr">
         <is>
-          <t>RAIANE DE SOUZA DANTAS</t>
+          <t>JURGEN WILLI LUDWIG VONNEILICH</t>
         </is>
       </c>
       <c r="C12" s="152" t="inlineStr">
         <is>
-          <t>513608124</t>
+          <t>513762567</t>
         </is>
       </c>
       <c r="D12" s="152" t="inlineStr"/>
@@ -6273,7 +6273,7 @@
       </c>
       <c r="F12" s="152" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G12" s="152" t="n">
@@ -6281,12 +6281,12 @@
       </c>
       <c r="H12" s="153" t="inlineStr">
         <is>
-          <t>MARIVALDO ARAGAO FERREIRA</t>
+          <t>GEFERSSON</t>
         </is>
       </c>
       <c r="I12" s="152" t="inlineStr">
         <is>
-          <t>513775191</t>
+          <t>2222</t>
         </is>
       </c>
       <c r="J12" s="152" t="inlineStr"/>
@@ -6295,7 +6295,7 @@
       </c>
       <c r="L12" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>D:30000|E:4126</t>
         </is>
       </c>
     </row>
@@ -6305,12 +6305,12 @@
       </c>
       <c r="B13" s="153" t="inlineStr">
         <is>
-          <t>JURGEN WILLI LUDWIG VONNEILICH</t>
+          <t>MOISES SANTOS DA SILVA</t>
         </is>
       </c>
       <c r="C13" s="152" t="inlineStr">
         <is>
-          <t>513762567</t>
+          <t>513760379</t>
         </is>
       </c>
       <c r="D13" s="152" t="inlineStr"/>
@@ -6319,7 +6319,7 @@
       </c>
       <c r="F13" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="G13" s="152" t="n">
@@ -6327,12 +6327,12 @@
       </c>
       <c r="H13" s="153" t="inlineStr">
         <is>
-          <t>GEFERSSON</t>
+          <t>GEANDRO SILVA</t>
         </is>
       </c>
       <c r="I13" s="152" t="inlineStr">
         <is>
-          <t>2222</t>
+          <t>444</t>
         </is>
       </c>
       <c r="J13" s="152" t="inlineStr"/>
@@ -6351,12 +6351,12 @@
       </c>
       <c r="B14" s="153" t="inlineStr">
         <is>
-          <t>MOISES SANTOS DA SILVA</t>
+          <t>LUCAS CERQUEIRA BATISTA</t>
         </is>
       </c>
       <c r="C14" s="152" t="inlineStr">
         <is>
-          <t>513760379</t>
+          <t>513782331</t>
         </is>
       </c>
       <c r="D14" s="152" t="inlineStr"/>
@@ -6365,7 +6365,7 @@
       </c>
       <c r="F14" s="152" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G14" s="152" t="n">
@@ -6373,12 +6373,12 @@
       </c>
       <c r="H14" s="153" t="inlineStr">
         <is>
-          <t>GEANDRO SILVA</t>
+          <t>ANTONIO SILVA</t>
         </is>
       </c>
       <c r="I14" s="152" t="inlineStr">
         <is>
-          <t>444</t>
+          <t>345435</t>
         </is>
       </c>
       <c r="J14" s="152" t="inlineStr"/>
@@ -6397,12 +6397,12 @@
       </c>
       <c r="B15" s="153" t="inlineStr">
         <is>
-          <t>LUCAS CERQUEIRA BATISTA</t>
+          <t>MARIVALDO ARAGAO FERREIRA</t>
         </is>
       </c>
       <c r="C15" s="152" t="inlineStr">
         <is>
-          <t>513782331</t>
+          <t>513775191</t>
         </is>
       </c>
       <c r="D15" s="152" t="inlineStr"/>
@@ -6417,25 +6417,17 @@
       <c r="G15" s="152" t="n">
         <v>13</v>
       </c>
-      <c r="H15" s="153" t="inlineStr">
-        <is>
-          <t>ANTONIO SILVA</t>
-        </is>
-      </c>
-      <c r="I15" s="152" t="inlineStr">
-        <is>
-          <t>345435</t>
-        </is>
-      </c>
-      <c r="J15" s="152" t="inlineStr"/>
+      <c r="H15" s="153" t="n"/>
+      <c r="I15" s="152" t="n"/>
+      <c r="J15" s="152" t="inlineStr">
+        <is>
+          <t>Soma</t>
+        </is>
+      </c>
       <c r="K15" s="154" t="n">
-        <v>192.61</v>
-      </c>
-      <c r="L15" s="152" t="inlineStr">
-        <is>
-          <t>D:30000|E:4126</t>
-        </is>
-      </c>
+        <v>2503.93</v>
+      </c>
+      <c r="L15" s="152" t="n"/>
     </row>
     <row r="16" ht="15" customHeight="1" s="78">
       <c r="A16" s="152" t="n">
@@ -6443,12 +6435,12 @@
       </c>
       <c r="B16" s="153" t="inlineStr">
         <is>
-          <t>MARIVALDO ARAGAO FERREIRA</t>
+          <t>KARINA LA FARINA NOGUEIRA BISPO</t>
         </is>
       </c>
       <c r="C16" s="152" t="inlineStr">
         <is>
-          <t>513775191</t>
+          <t>513790578</t>
         </is>
       </c>
       <c r="D16" s="152" t="inlineStr"/>
@@ -6457,7 +6449,7 @@
       </c>
       <c r="F16" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>100E / 48,65D</t>
         </is>
       </c>
       <c r="G16" s="152" t="n"/>
@@ -6465,11 +6457,11 @@
       <c r="I16" s="152" t="n"/>
       <c r="J16" s="152" t="inlineStr">
         <is>
-          <t>Soma</t>
+          <t>Psicólogo</t>
         </is>
       </c>
       <c r="K16" s="154" t="n">
-        <v>2503.93</v>
+        <v>825.5</v>
       </c>
       <c r="L16" s="152" t="n"/>
     </row>
@@ -6479,12 +6471,12 @@
       </c>
       <c r="B17" s="153" t="inlineStr">
         <is>
-          <t>KARINA LA FARINA NOGUEIRA BISPO</t>
+          <t>DIOGENES FREDERICO CONCEICAO SILVA</t>
         </is>
       </c>
       <c r="C17" s="152" t="inlineStr">
         <is>
-          <t>513790578</t>
+          <t>513721847</t>
         </is>
       </c>
       <c r="D17" s="152" t="inlineStr"/>
@@ -6493,7 +6485,7 @@
       </c>
       <c r="F17" s="152" t="inlineStr">
         <is>
-          <t>100E / 48,65D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G17" s="152" t="n"/>
@@ -6501,11 +6493,11 @@
       <c r="I17" s="152" t="n"/>
       <c r="J17" s="152" t="inlineStr">
         <is>
-          <t>Psicólogo</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="K17" s="154" t="n">
-        <v>825.5</v>
+        <v>1678.43</v>
       </c>
       <c r="L17" s="152" t="n"/>
     </row>
@@ -6515,12 +6507,12 @@
       </c>
       <c r="B18" s="153" t="inlineStr">
         <is>
-          <t>DIOGENES FREDERICO CONCEICAO SILVA</t>
+          <t>EVANILDES ALVES DE FIGUEREDO</t>
         </is>
       </c>
       <c r="C18" s="152" t="inlineStr">
         <is>
-          <t>513721847</t>
+          <t>513782693</t>
         </is>
       </c>
       <c r="D18" s="152" t="inlineStr"/>
@@ -6535,14 +6527,8 @@
       <c r="G18" s="152" t="n"/>
       <c r="H18" s="152" t="n"/>
       <c r="I18" s="152" t="n"/>
-      <c r="J18" s="152" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="K18" s="154" t="n">
-        <v>1678.43</v>
-      </c>
+      <c r="J18" s="152" t="n"/>
+      <c r="K18" s="154" t="n"/>
       <c r="L18" s="152" t="n"/>
     </row>
     <row r="19" ht="15" customHeight="1" s="78">
@@ -6551,12 +6537,12 @@
       </c>
       <c r="B19" s="153" t="inlineStr">
         <is>
-          <t>EVANILDES ALVES DE FIGUEREDO</t>
+          <t>VICTOR RAFAEL ANDRADE O P DE GUIMARAES SOUZA</t>
         </is>
       </c>
       <c r="C19" s="152" t="inlineStr">
         <is>
-          <t>513782693</t>
+          <t>513773401</t>
         </is>
       </c>
       <c r="D19" s="152" t="inlineStr"/>
@@ -6565,14 +6551,14 @@
       </c>
       <c r="F19" s="152" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G19" s="152" t="n"/>
       <c r="H19" s="152" t="n"/>
       <c r="I19" s="152" t="n"/>
       <c r="J19" s="152" t="n"/>
-      <c r="K19" s="155" t="n"/>
+      <c r="K19" s="154" t="n"/>
       <c r="L19" s="152" t="n"/>
     </row>
     <row r="20" ht="15" customHeight="1" s="78">
@@ -6581,12 +6567,12 @@
       </c>
       <c r="B20" s="153" t="inlineStr">
         <is>
-          <t>VICTOR RAFAEL ANDRADE O P DE GUIMARAES SOUZA</t>
+          <t>VERA LUCIA SILVA TAVARES</t>
         </is>
       </c>
       <c r="C20" s="152" t="inlineStr">
         <is>
-          <t>513773401</t>
+          <t>513797287</t>
         </is>
       </c>
       <c r="D20" s="152" t="inlineStr"/>
@@ -6595,14 +6581,14 @@
       </c>
       <c r="F20" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="G20" s="152" t="n"/>
       <c r="H20" s="152" t="n"/>
       <c r="I20" s="152" t="n"/>
       <c r="J20" s="152" t="n"/>
-      <c r="K20" s="155" t="n"/>
+      <c r="K20" s="154" t="n"/>
       <c r="L20" s="152" t="n"/>
     </row>
     <row r="21" ht="15" customHeight="1" s="78">
@@ -6611,12 +6597,12 @@
       </c>
       <c r="B21" s="153" t="inlineStr">
         <is>
-          <t>VERA LUCIA SILVA TAVARES</t>
+          <t>BRISA CARVALHO ROCHA HITA</t>
         </is>
       </c>
       <c r="C21" s="152" t="inlineStr">
         <is>
-          <t>513797287</t>
+          <t>14091389</t>
         </is>
       </c>
       <c r="D21" s="152" t="inlineStr"/>
@@ -6641,12 +6627,12 @@
       </c>
       <c r="B22" s="153" t="inlineStr">
         <is>
-          <t>BRISA CARVALHO ROCHA HITA</t>
+          <t>FERNANDA MIGUEZ SENA DE JESUS</t>
         </is>
       </c>
       <c r="C22" s="152" t="inlineStr">
         <is>
-          <t>14091389</t>
+          <t>513791549</t>
         </is>
       </c>
       <c r="D22" s="152" t="inlineStr"/>
@@ -6655,14 +6641,14 @@
       </c>
       <c r="F22" s="152" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G22" s="152" t="n"/>
       <c r="H22" s="152" t="n"/>
       <c r="I22" s="152" t="n"/>
       <c r="J22" s="152" t="n"/>
-      <c r="K22" s="156" t="n"/>
+      <c r="K22" s="155" t="n"/>
       <c r="L22" s="152" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" s="78">
@@ -6671,12 +6657,12 @@
       </c>
       <c r="B23" s="153" t="inlineStr">
         <is>
-          <t>FERNANDA MIGUEZ SENA DE JESUS</t>
+          <t>GEFERSSON</t>
         </is>
       </c>
       <c r="C23" s="152" t="inlineStr">
         <is>
-          <t>513791549</t>
+          <t>2222</t>
         </is>
       </c>
       <c r="D23" s="152" t="inlineStr"/>
@@ -6685,7 +6671,7 @@
       </c>
       <c r="F23" s="152" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>D:30000|E:4126</t>
         </is>
       </c>
       <c r="G23" s="152" t="n"/>
@@ -6701,12 +6687,12 @@
       </c>
       <c r="B24" s="153" t="inlineStr">
         <is>
-          <t>GEFERSSON</t>
+          <t>GEANDRO SILVA</t>
         </is>
       </c>
       <c r="C24" s="152" t="inlineStr">
         <is>
-          <t>2222</t>
+          <t>444</t>
         </is>
       </c>
       <c r="D24" s="152" t="inlineStr"/>
@@ -6722,7 +6708,7 @@
       <c r="H24" s="152" t="n"/>
       <c r="I24" s="152" t="n"/>
       <c r="J24" s="152" t="n"/>
-      <c r="K24" s="157" t="n"/>
+      <c r="K24" s="156" t="n"/>
       <c r="L24" s="152" t="n"/>
     </row>
     <row r="25" ht="15" customHeight="1" s="78">
@@ -6731,12 +6717,12 @@
       </c>
       <c r="B25" s="153" t="inlineStr">
         <is>
-          <t>GEANDRO SILVA</t>
+          <t>LUCIANO</t>
         </is>
       </c>
       <c r="C25" s="152" t="inlineStr">
         <is>
-          <t>444</t>
+          <t>999</t>
         </is>
       </c>
       <c r="D25" s="152" t="inlineStr"/>
@@ -6745,14 +6731,14 @@
       </c>
       <c r="F25" s="152" t="inlineStr">
         <is>
-          <t>D:30000|E:4126</t>
+          <t>D</t>
         </is>
       </c>
       <c r="G25" s="152" t="n"/>
       <c r="H25" s="152" t="n"/>
-      <c r="I25" s="158" t="n"/>
+      <c r="I25" s="152" t="n"/>
       <c r="J25" s="152" t="n"/>
-      <c r="K25" s="157" t="n"/>
+      <c r="K25" s="155" t="n"/>
       <c r="L25" s="152" t="n"/>
     </row>
     <row r="26" ht="15" customHeight="1" s="78">
@@ -6761,12 +6747,12 @@
       </c>
       <c r="B26" s="153" t="inlineStr">
         <is>
-          <t>LUCIANO</t>
+          <t>ANTONIO SILVA</t>
         </is>
       </c>
       <c r="C26" s="152" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>345435</t>
         </is>
       </c>
       <c r="D26" s="152" t="inlineStr"/>
@@ -6775,12 +6761,12 @@
       </c>
       <c r="F26" s="152" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="G26" s="156" t="n"/>
+          <t>D:30000|E:4126</t>
+        </is>
+      </c>
+      <c r="G26" s="152" t="n"/>
       <c r="H26" s="152" t="n"/>
-      <c r="I26" s="158" t="n"/>
+      <c r="I26" s="152" t="n"/>
       <c r="J26" s="152" t="n"/>
       <c r="K26" s="157" t="n"/>
       <c r="L26" s="152" t="n"/>
@@ -6789,30 +6775,22 @@
       <c r="A27" s="152" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="153" t="inlineStr">
-        <is>
-          <t>ANTONIO SILVA</t>
-        </is>
-      </c>
-      <c r="C27" s="152" t="inlineStr">
-        <is>
-          <t>345435</t>
-        </is>
-      </c>
-      <c r="D27" s="152" t="inlineStr"/>
+      <c r="B27" s="153" t="n"/>
+      <c r="C27" s="152" t="n"/>
+      <c r="D27" s="152" t="inlineStr">
+        <is>
+          <t>Soma</t>
+        </is>
+      </c>
       <c r="E27" s="154" t="n">
-        <v>148.65</v>
-      </c>
-      <c r="F27" s="152" t="inlineStr">
-        <is>
-          <t>D:30000|E:4126</t>
-        </is>
-      </c>
+        <v>3716.25</v>
+      </c>
+      <c r="F27" s="152" t="n"/>
       <c r="G27" s="152" t="n"/>
       <c r="H27" s="152" t="n"/>
-      <c r="I27" s="152" t="n"/>
+      <c r="I27" s="158" t="n"/>
       <c r="J27" s="152" t="n"/>
-      <c r="K27" s="152" t="n"/>
+      <c r="K27" s="157" t="n"/>
       <c r="L27" s="152" t="n"/>
     </row>
     <row r="28" ht="15" customHeight="1" s="78">
@@ -6821,11 +6799,11 @@
       <c r="C28" s="152" t="n"/>
       <c r="D28" s="152" t="inlineStr">
         <is>
-          <t>Soma</t>
+          <t>Médico</t>
         </is>
       </c>
       <c r="E28" s="154" t="n">
-        <v>3716.25</v>
+        <v>1225</v>
       </c>
       <c r="F28" s="152" t="n"/>
       <c r="G28" s="152" t="n"/>
@@ -6841,38 +6819,32 @@
       <c r="C29" s="152" t="n"/>
       <c r="D29" s="152" t="inlineStr">
         <is>
-          <t>Médico</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="E29" s="154" t="n">
-        <v>1225</v>
+        <v>2491.25</v>
       </c>
       <c r="F29" s="152" t="n"/>
-      <c r="G29" s="152" t="n"/>
+      <c r="G29" s="156" t="n"/>
       <c r="H29" s="152" t="n"/>
-      <c r="I29" s="152" t="n"/>
+      <c r="I29" s="158" t="n"/>
       <c r="J29" s="152" t="n"/>
-      <c r="K29" s="152" t="n"/>
+      <c r="K29" s="157" t="n"/>
       <c r="L29" s="152" t="n"/>
     </row>
     <row r="30" ht="14.25" customHeight="1" s="78">
       <c r="A30" s="152" t="n"/>
       <c r="B30" s="152" t="n"/>
       <c r="C30" s="152" t="n"/>
-      <c r="D30" s="152" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E30" s="154" t="n">
-        <v>2491.25</v>
-      </c>
+      <c r="D30" s="152" t="n"/>
+      <c r="E30" s="154" t="n"/>
       <c r="F30" s="152" t="n"/>
       <c r="G30" s="152" t="n"/>
       <c r="H30" s="152" t="n"/>
       <c r="I30" s="152" t="n"/>
       <c r="J30" s="152" t="n"/>
-      <c r="K30" s="155" t="n"/>
+      <c r="K30" s="152" t="n"/>
       <c r="L30" s="152" t="n"/>
     </row>
     <row r="31" ht="14.25" customHeight="1" s="78">
@@ -6916,6 +6888,62 @@
       <c r="J33" s="152" t="n"/>
       <c r="K33" s="152" t="n"/>
       <c r="L33" s="152" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="152" t="n"/>
+      <c r="B34" s="152" t="n"/>
+      <c r="C34" s="152" t="n"/>
+      <c r="D34" s="152" t="n"/>
+      <c r="E34" s="154" t="n"/>
+      <c r="F34" s="152" t="n"/>
+      <c r="G34" s="152" t="n"/>
+      <c r="H34" s="152" t="n"/>
+      <c r="I34" s="152" t="n"/>
+      <c r="J34" s="152" t="n"/>
+      <c r="K34" s="155" t="n"/>
+      <c r="L34" s="152" t="n"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="152" t="n"/>
+      <c r="B35" s="152" t="n"/>
+      <c r="C35" s="152" t="n"/>
+      <c r="D35" s="152" t="n"/>
+      <c r="E35" s="154" t="n"/>
+      <c r="F35" s="152" t="n"/>
+      <c r="G35" s="152" t="n"/>
+      <c r="H35" s="152" t="n"/>
+      <c r="I35" s="152" t="n"/>
+      <c r="J35" s="152" t="n"/>
+      <c r="K35" s="152" t="n"/>
+      <c r="L35" s="152" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="152" t="n"/>
+      <c r="B36" s="152" t="n"/>
+      <c r="C36" s="152" t="n"/>
+      <c r="D36" s="152" t="n"/>
+      <c r="E36" s="154" t="n"/>
+      <c r="F36" s="152" t="n"/>
+      <c r="G36" s="152" t="n"/>
+      <c r="H36" s="152" t="n"/>
+      <c r="I36" s="152" t="n"/>
+      <c r="J36" s="152" t="n"/>
+      <c r="K36" s="152" t="n"/>
+      <c r="L36" s="152" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="152" t="n"/>
+      <c r="B37" s="152" t="n"/>
+      <c r="C37" s="152" t="n"/>
+      <c r="D37" s="152" t="n"/>
+      <c r="E37" s="154" t="n"/>
+      <c r="F37" s="152" t="n"/>
+      <c r="G37" s="152" t="n"/>
+      <c r="H37" s="152" t="n"/>
+      <c r="I37" s="152" t="n"/>
+      <c r="J37" s="152" t="n"/>
+      <c r="K37" s="152" t="n"/>
+      <c r="L37" s="152" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
commit para testes graficos
</commit_message>
<xml_diff>
--- a/CAMPSSA.xlsx
+++ b/CAMPSSA.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="01.10" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="02.10" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="03.10" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="04.10" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10.10" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="15.10" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="16.10" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="17.10" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planilha10" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planilha11" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planilha12" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planilha13" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contas Fechamento" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planilha15" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet nova" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nuevo" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="01.10" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="02.10" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="03.10" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="04.10" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="10.10" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="15.10" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="16.10" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="17.10" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Planilha10" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Planilha11" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Planilha12" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Planilha13" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Contas Fechamento" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Planilha15" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="sheet nova" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="nuevo" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" calcMode="manual" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -908,7 +908,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
@@ -933,24 +933,24 @@
     <row r="1" ht="15" customHeight="1" s="8">
       <c r="A1" s="111" t="inlineStr">
         <is>
-          <t>(Usuário) Atendimento Médico 25/11/2024</t>
-        </is>
-      </c>
-      <c r="B1" s="121" t="n"/>
-      <c r="C1" s="121" t="n"/>
-      <c r="D1" s="121" t="n"/>
-      <c r="E1" s="121" t="n"/>
-      <c r="F1" s="122" t="n"/>
+          <t>(Usuário) Atendimento Médico 29/11/2024</t>
+        </is>
+      </c>
+      <c r="B1" s="112" t="n"/>
+      <c r="C1" s="112" t="n"/>
+      <c r="D1" s="112" t="n"/>
+      <c r="E1" s="112" t="n"/>
+      <c r="F1" s="113" t="n"/>
       <c r="G1" s="111" t="inlineStr">
         <is>
-          <t>(Usuário) Atendimento Psicológico 25/11/2024</t>
-        </is>
-      </c>
-      <c r="H1" s="121" t="n"/>
-      <c r="I1" s="121" t="n"/>
-      <c r="J1" s="121" t="n"/>
-      <c r="K1" s="121" t="n"/>
-      <c r="L1" s="122" t="n"/>
+          <t>(Usuário) Atendimento Psicológico 29/11/2024</t>
+        </is>
+      </c>
+      <c r="H1" s="112" t="n"/>
+      <c r="I1" s="112" t="n"/>
+      <c r="J1" s="112" t="n"/>
+      <c r="K1" s="112" t="n"/>
+      <c r="L1" s="113" t="n"/>
     </row>
     <row r="2" ht="15" customHeight="1" s="8">
       <c r="A2" s="111" t="inlineStr">
@@ -1856,7 +1856,7 @@
           <t>36463</t>
         </is>
       </c>
-      <c r="D21" s="114" t="n"/>
+      <c r="D21" s="114" t="inlineStr"/>
       <c r="E21" s="116" t="n">
         <v>148.65</v>
       </c>
@@ -1902,7 +1902,7 @@
           <t>421</t>
         </is>
       </c>
-      <c r="D22" s="114" t="n"/>
+      <c r="D22" s="114" t="inlineStr"/>
       <c r="E22" s="116" t="n">
         <v>148.65</v>
       </c>
@@ -1948,7 +1948,7 @@
           <t>6532</t>
         </is>
       </c>
-      <c r="D23" s="114" t="n"/>
+      <c r="D23" s="114" t="inlineStr"/>
       <c r="E23" s="116" t="n">
         <v>148.65</v>
       </c>
@@ -1994,7 +1994,7 @@
           <t>6523</t>
         </is>
       </c>
-      <c r="D24" s="114" t="n"/>
+      <c r="D24" s="114" t="inlineStr"/>
       <c r="E24" s="116" t="n">
         <v>148.65</v>
       </c>
@@ -2030,17 +2030,25 @@
       <c r="A25" s="114" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="115" t="n"/>
-      <c r="C25" s="114" t="n"/>
-      <c r="D25" s="114" t="inlineStr">
-        <is>
-          <t>Soma</t>
-        </is>
-      </c>
+      <c r="B25" s="115" t="inlineStr">
+        <is>
+          <t>TECA</t>
+        </is>
+      </c>
+      <c r="C25" s="114" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="D25" s="114" t="inlineStr"/>
       <c r="E25" s="116" t="n">
-        <v>3716.25</v>
-      </c>
-      <c r="F25" s="114" t="n"/>
+        <v>148.65</v>
+      </c>
+      <c r="F25" s="114" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
       <c r="G25" s="114" t="n">
         <v>23</v>
       </c>
@@ -2065,18 +2073,16 @@
       </c>
     </row>
     <row r="26" ht="15" customHeight="1" s="8">
-      <c r="A26" s="114" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" s="115" t="n"/>
+      <c r="A26" s="114" t="n"/>
+      <c r="B26" s="114" t="n"/>
       <c r="C26" s="114" t="n"/>
       <c r="D26" s="114" t="inlineStr">
         <is>
-          <t>Médico</t>
+          <t>Soma</t>
         </is>
       </c>
       <c r="E26" s="116" t="n">
-        <v>1225</v>
+        <v>3418.95</v>
       </c>
       <c r="F26" s="114" t="n"/>
       <c r="G26" s="114" t="n">
@@ -2092,7 +2098,7 @@
           <t>6523</t>
         </is>
       </c>
-      <c r="J26" s="114" t="n"/>
+      <c r="J26" s="114" t="inlineStr"/>
       <c r="K26" s="116" t="n">
         <v>192.61</v>
       </c>
@@ -2103,52 +2109,64 @@
       </c>
     </row>
     <row r="27" ht="15" customHeight="1" s="8">
-      <c r="A27" s="114" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" s="115" t="n"/>
+      <c r="A27" s="114" t="n"/>
+      <c r="B27" s="114" t="n"/>
       <c r="C27" s="114" t="n"/>
       <c r="D27" s="114" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Médico</t>
         </is>
       </c>
       <c r="E27" s="116" t="n">
-        <v>2491.25</v>
+        <v>1127</v>
       </c>
       <c r="F27" s="114" t="n"/>
       <c r="G27" s="114" t="n">
         <v>25</v>
       </c>
-      <c r="H27" s="115" t="n"/>
-      <c r="I27" s="114" t="n"/>
-      <c r="J27" s="114" t="inlineStr">
-        <is>
-          <t>Soma</t>
-        </is>
-      </c>
+      <c r="H27" s="115" t="inlineStr">
+        <is>
+          <t>TECA</t>
+        </is>
+      </c>
+      <c r="I27" s="114" t="inlineStr">
+        <is>
+          <t>2222</t>
+        </is>
+      </c>
+      <c r="J27" s="114" t="inlineStr"/>
       <c r="K27" s="116" t="n">
-        <v>4815.25</v>
-      </c>
-      <c r="L27" s="114" t="n"/>
+        <v>192.61</v>
+      </c>
+      <c r="L27" s="114" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="114" t="n"/>
       <c r="B28" s="114" t="n"/>
       <c r="C28" s="114" t="n"/>
-      <c r="D28" s="114" t="n"/>
-      <c r="E28" s="116" t="n"/>
+      <c r="D28" s="114" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E28" s="116" t="n">
+        <v>2291.95</v>
+      </c>
       <c r="F28" s="114" t="n"/>
       <c r="G28" s="114" t="n"/>
       <c r="H28" s="114" t="n"/>
       <c r="I28" s="114" t="n"/>
       <c r="J28" s="114" t="inlineStr">
         <is>
-          <t>Psicólogo</t>
+          <t>Soma</t>
         </is>
       </c>
       <c r="K28" s="116" t="n">
-        <v>1587.5</v>
+        <v>4815.25</v>
       </c>
       <c r="L28" s="114" t="n"/>
     </row>
@@ -2164,11 +2182,11 @@
       <c r="I29" s="114" t="n"/>
       <c r="J29" s="114" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="K29" s="117" t="n">
-        <v>3227.75</v>
+          <t>Psicólogo</t>
+        </is>
+      </c>
+      <c r="K29" s="116" t="n">
+        <v>1587.5</v>
       </c>
       <c r="L29" s="114" t="n"/>
     </row>
@@ -2181,9 +2199,15 @@
       <c r="F30" s="114" t="n"/>
       <c r="G30" s="114" t="n"/>
       <c r="H30" s="114" t="n"/>
-      <c r="I30" s="118" t="n"/>
-      <c r="J30" s="114" t="n"/>
-      <c r="K30" s="117" t="n"/>
+      <c r="I30" s="114" t="n"/>
+      <c r="J30" s="114" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K30" s="116" t="n">
+        <v>3227.75</v>
+      </c>
       <c r="L30" s="114" t="n"/>
     </row>
     <row r="31">
@@ -2193,9 +2217,9 @@
       <c r="D31" s="114" t="n"/>
       <c r="E31" s="116" t="n"/>
       <c r="F31" s="114" t="n"/>
-      <c r="G31" s="119" t="n"/>
+      <c r="G31" s="114" t="n"/>
       <c r="H31" s="114" t="n"/>
-      <c r="I31" s="118" t="n"/>
+      <c r="I31" s="114" t="n"/>
       <c r="J31" s="114" t="n"/>
       <c r="K31" s="117" t="n"/>
       <c r="L31" s="114" t="n"/>
@@ -2205,13 +2229,13 @@
       <c r="B32" s="114" t="n"/>
       <c r="C32" s="114" t="n"/>
       <c r="D32" s="114" t="n"/>
-      <c r="E32" s="120" t="n"/>
+      <c r="E32" s="116" t="n"/>
       <c r="F32" s="114" t="n"/>
       <c r="G32" s="114" t="n"/>
       <c r="H32" s="114" t="n"/>
-      <c r="I32" s="114" t="n"/>
+      <c r="I32" s="118" t="n"/>
       <c r="J32" s="114" t="n"/>
-      <c r="K32" s="116" t="n"/>
+      <c r="K32" s="117" t="n"/>
       <c r="L32" s="114" t="n"/>
     </row>
     <row r="33">
@@ -2219,13 +2243,13 @@
       <c r="B33" s="114" t="n"/>
       <c r="C33" s="114" t="n"/>
       <c r="D33" s="114" t="n"/>
-      <c r="E33" s="114" t="n"/>
+      <c r="E33" s="116" t="n"/>
       <c r="F33" s="114" t="n"/>
-      <c r="G33" s="114" t="n"/>
+      <c r="G33" s="119" t="n"/>
       <c r="H33" s="114" t="n"/>
-      <c r="I33" s="114" t="n"/>
+      <c r="I33" s="118" t="n"/>
       <c r="J33" s="114" t="n"/>
-      <c r="K33" s="116" t="n"/>
+      <c r="K33" s="117" t="n"/>
       <c r="L33" s="114" t="n"/>
     </row>
     <row r="34">
@@ -2233,7 +2257,7 @@
       <c r="B34" s="114" t="n"/>
       <c r="C34" s="114" t="n"/>
       <c r="D34" s="114" t="n"/>
-      <c r="E34" s="114" t="n"/>
+      <c r="E34" s="120" t="n"/>
       <c r="F34" s="114" t="n"/>
       <c r="G34" s="114" t="n"/>
       <c r="H34" s="114" t="n"/>
@@ -2323,8 +2347,36 @@
       <c r="H40" s="114" t="n"/>
       <c r="I40" s="114" t="n"/>
       <c r="J40" s="114" t="n"/>
-      <c r="K40" s="114" t="n"/>
+      <c r="K40" s="116" t="n"/>
       <c r="L40" s="114" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="114" t="n"/>
+      <c r="B41" s="114" t="n"/>
+      <c r="C41" s="114" t="n"/>
+      <c r="D41" s="114" t="n"/>
+      <c r="E41" s="114" t="n"/>
+      <c r="F41" s="114" t="n"/>
+      <c r="G41" s="114" t="n"/>
+      <c r="H41" s="114" t="n"/>
+      <c r="I41" s="114" t="n"/>
+      <c r="J41" s="114" t="n"/>
+      <c r="K41" s="116" t="n"/>
+      <c r="L41" s="114" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="114" t="n"/>
+      <c r="B42" s="114" t="n"/>
+      <c r="C42" s="114" t="n"/>
+      <c r="D42" s="114" t="n"/>
+      <c r="E42" s="114" t="n"/>
+      <c r="F42" s="114" t="n"/>
+      <c r="G42" s="114" t="n"/>
+      <c r="H42" s="114" t="n"/>
+      <c r="I42" s="114" t="n"/>
+      <c r="J42" s="114" t="n"/>
+      <c r="K42" s="114" t="n"/>
+      <c r="L42" s="114" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>